<commit_message>
- added this week and next week indicators to the events - moved drivers location - prepared to read events_selection.xlsx file to compare against events list
</commit_message>
<xml_diff>
--- a/events_selection.xlsx
+++ b/events_selection.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD4129C-FC48-4821-B649-D9ED0C988A99}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9218F2C-073C-4E84-B73C-5252787CCB1E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22212" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Events" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Events!$A$1:$F$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Events!$B$1:$F$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -70,12 +70,6 @@
     <t>Thursday</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>Pilates</t>
   </si>
   <si>
@@ -94,9 +88,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Go? (Y/N)</t>
-  </si>
-  <si>
     <t>Week</t>
   </si>
   <si>
@@ -107,6 +98,15 @@
   </si>
   <si>
     <t>Event Name</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Go?</t>
   </si>
 </sst>
 </file>
@@ -114,7 +114,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -168,69 +168,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -240,6 +184,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6565"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -574,14 +523,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.77734375" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="41.77734375" customWidth="1"/>
     <col min="3" max="3" width="12.77734375" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" customWidth="1"/>
     <col min="5" max="5" width="13.77734375" customWidth="1"/>
@@ -589,37 +536,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>22</v>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -629,17 +576,17 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -649,17 +596,17 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -669,17 +616,17 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -689,17 +636,17 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
@@ -709,17 +656,17 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -729,17 +676,17 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -749,17 +696,17 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
@@ -769,17 +716,17 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -789,17 +736,17 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -809,17 +756,17 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
@@ -829,17 +776,17 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -849,17 +796,17 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
@@ -869,17 +816,17 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -889,17 +836,17 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -909,17 +856,17 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
@@ -929,17 +876,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F17" xr:uid="{360C01DB-4E7B-421A-92F4-06BCA4EC7D7C}"/>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$B:$B = "Y"</formula>
+  <autoFilter ref="B1:F17" xr:uid="{360C01DB-4E7B-421A-92F4-06BCA4EC7D7C}"/>
+  <conditionalFormatting sqref="A1:F1048576">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$A1="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:F1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$B1 = "Y"</formula>
-    </cfRule>
-  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A17" xr:uid="{28D91E24-F200-4948-BB96-A4892019C624}">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
- can read events from events_selection.xlsx - added sanity checks in main - tuple for weeks added (skipping creating an object)
</commit_message>
<xml_diff>
--- a/events_selection.xlsx
+++ b/events_selection.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9218F2C-073C-4E84-B73C-5252787CCB1E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAD50F8-642C-495A-89A7-A0D093FF2CFC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22212" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -523,7 +523,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
- All event lists are now Event class objects - Event class expanded to have a second constructor and object equality added - Intersection between event lists added
</commit_message>
<xml_diff>
--- a/events_selection.xlsx
+++ b/events_selection.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAD50F8-642C-495A-89A7-A0D093FF2CFC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E3082B-2049-4AFE-BA72-F6A2582AB12E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22212" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21780" yWindow="-108" windowWidth="21888" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="29">
   <si>
     <t>Class</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>Go?</t>
+  </si>
+  <si>
+    <t>Book of the Month Giveaway: The Art of Keeping Secrets</t>
+  </si>
+  <si>
+    <t>Book</t>
   </si>
 </sst>
 </file>
@@ -116,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +134,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -521,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -877,8 +889,49 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="5">
+        <v>4.1666666666666699E-2</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B1:F17" xr:uid="{360C01DB-4E7B-421A-92F4-06BCA4EC7D7C}"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A1:F1048576">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$A1="Yes"</formula>

</xml_diff>

<commit_message>
Successfully RSVP'ed to an event
</commit_message>
<xml_diff>
--- a/events_selection.xlsx
+++ b/events_selection.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E3082B-2049-4AFE-BA72-F6A2582AB12E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26FF074-60F0-4BAB-9468-4B82D0AB4B46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21780" yWindow="-108" windowWidth="21888" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="31">
   <si>
     <t>Class</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>Book</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Shen Yun: 5,000 years of civilisation live on stage</t>
   </si>
 </sst>
 </file>
@@ -536,7 +542,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -911,16 +917,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
@@ -937,7 +943,7 @@
       <formula>$A1="Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A17" xr:uid="{28D91E24-F200-4948-BB96-A4892019C624}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>

</xml_diff>